<commit_message>
changed DriverManager.java massive updates
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/pseudo_candy_company.xlsx
+++ b/src/test/resources/test-data/pseudo_candy_company.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hui Yang\eclipse-workspace-2\demo-qa-web-junit-5\src\test\resources\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC5D1ED-3361-48BA-B5DA-3EF1342819A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A7CB36B-993D-4719-9545-5786EA9F82D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="employees" sheetId="1" r:id="rId1"/>
@@ -439,7 +439,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
@@ -556,7 +556,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78EB05FC-D0CC-4B08-BEBF-CDAAB1182372}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>